<commit_message>
fix: fix multi-flight route assign template
Import requires From, To and Route. However, Route was not in the template
</commit_message>
<xml_diff>
--- a/public/import_multi_flights_assign_routes_template.xlsx
+++ b/public/import_multi_flights_assign_routes_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daveroverts/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D9AEFAA-9B6E-4E41-B082-3AE58C2DB6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC5A770-F41B-8644-9336-D8882EC41F41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18600" yWindow="7000" windowWidth="29040" windowHeight="15840" xr2:uid="{D04AF5E1-FD0B-423F-91F9-BDC72DF41FA8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>From</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>Route</t>
   </si>
 </sst>
 </file>
@@ -91,9 +94,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -408,7 +412,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91403348-4099-4258-BDAA-3E7E76500E16}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -420,7 +424,7 @@
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -428,6 +432,9 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>